<commit_message>
Eliminated PD´s and updated with Demo values
</commit_message>
<xml_diff>
--- a/PD Data.xlsx
+++ b/PD Data.xlsx
@@ -1867,52 +1867,55 @@
         <v>25</v>
       </c>
       <c r="B26" s="2">
-        <v>3.7828212999999999E-2</v>
-      </c>
-      <c r="C26" s="4">
-        <v>1.97843506E-2</v>
-      </c>
-      <c r="D26" s="4">
-        <v>9.7609527599999996E-2</v>
+        <v>1</v>
+      </c>
+      <c r="C26" s="2">
+        <v>1</v>
+      </c>
+      <c r="D26" s="2">
+        <v>1</v>
       </c>
       <c r="E26" s="2">
-        <v>2.9311558433738547E-2</v>
+        <v>1</v>
       </c>
       <c r="F26" s="2">
-        <v>2.0619290419732848E-2</v>
+        <v>1</v>
       </c>
       <c r="G26" s="2">
-        <v>5.0512427072871728E-2</v>
+        <v>1</v>
       </c>
       <c r="H26" s="2">
-        <v>5.5651488964873042E-2</v>
-      </c>
-      <c r="I26">
-        <v>5.0496761000000001E-2</v>
-      </c>
-      <c r="K26">
-        <v>1.4824207492795389E-2</v>
-      </c>
-      <c r="L26">
-        <v>2.1996120483233045E-2</v>
-      </c>
-      <c r="M26">
-        <v>7.755073424842937E-2</v>
-      </c>
-      <c r="N26">
-        <v>1.9706419673505626E-2</v>
-      </c>
-      <c r="O26">
-        <v>3.0212619649756561E-2</v>
-      </c>
-      <c r="P26">
-        <v>0.10109996947658061</v>
-      </c>
-      <c r="Q26">
-        <v>2.0561907294159354E-2</v>
-      </c>
-      <c r="R26">
-        <v>8.0890908083550341E-3</v>
+        <v>1</v>
+      </c>
+      <c r="I26" s="2">
+        <v>1</v>
+      </c>
+      <c r="J26" s="2">
+        <v>1</v>
+      </c>
+      <c r="K26" s="2">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="N26" s="2">
+        <v>1</v>
+      </c>
+      <c r="O26" s="2">
+        <v>1</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q26" s="2">
+        <v>1</v>
+      </c>
+      <c r="R26" s="2">
+        <v>1</v>
       </c>
       <c r="DC26" s="3"/>
     </row>
@@ -1921,52 +1924,55 @@
         <v>26</v>
       </c>
       <c r="B27" s="2">
-        <v>5.3876535400000002E-2</v>
-      </c>
-      <c r="C27" s="4">
-        <v>2.7577301799999999E-2</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0.1121670812</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D27" s="2">
+        <v>1.1000000000000001</v>
       </c>
       <c r="E27" s="2">
-        <v>3.0769625403455458E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F27" s="2">
-        <v>2.3760060323469216E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G27" s="2">
-        <v>5.7405158709543463E-2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H27" s="2">
-        <v>5.9305681561663152E-2</v>
-      </c>
-      <c r="I27" s="1">
-        <v>5.15443685E-2</v>
-      </c>
-      <c r="K27">
-        <v>1.8351848246490471E-2</v>
-      </c>
-      <c r="L27">
-        <v>2.6125981726305574E-2</v>
-      </c>
-      <c r="M27">
-        <v>7.1599005903361393E-2</v>
-      </c>
-      <c r="N27">
-        <v>3.0516030155502243E-2</v>
-      </c>
-      <c r="O27">
-        <v>3.5779789517707279E-2</v>
-      </c>
-      <c r="P27">
-        <v>0.10935501934858376</v>
-      </c>
-      <c r="Q27">
-        <v>2.4683739586547362E-2</v>
-      </c>
-      <c r="R27">
-        <v>1.3264517415912435E-2</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="I27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="J27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="M27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="N27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="O27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="P27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="Q27" s="2">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="R27" s="2">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:715" x14ac:dyDescent="0.25">
@@ -1974,55 +1980,55 @@
         <v>27</v>
       </c>
       <c r="B28" s="2">
-        <v>7.1957088500000002E-2</v>
-      </c>
-      <c r="C28" s="4">
-        <v>4.55677814E-2</v>
-      </c>
-      <c r="D28" s="4">
-        <v>0.140138716</v>
+        <v>1.2</v>
+      </c>
+      <c r="C28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>1.2</v>
       </c>
       <c r="E28" s="2">
-        <v>3.3073924963890236E-2</v>
+        <v>1.2</v>
       </c>
       <c r="F28" s="2">
-        <v>2.5814117858695543E-2</v>
+        <v>1.2</v>
       </c>
       <c r="G28" s="2">
-        <v>6.4421892535952874E-2</v>
+        <v>1.2</v>
       </c>
       <c r="H28" s="2">
-        <v>6.3769693004155456E-2</v>
-      </c>
-      <c r="I28">
-        <v>5.34110052E-2</v>
-      </c>
-      <c r="J28">
-        <v>2.1908755117027067E-2</v>
-      </c>
-      <c r="K28">
-        <v>2.1458635265508761E-2</v>
-      </c>
-      <c r="L28">
-        <v>3.2445177768417245E-2</v>
-      </c>
-      <c r="M28">
-        <v>7.0084408420401631E-2</v>
-      </c>
-      <c r="N28">
-        <v>3.9542113998391852E-2</v>
-      </c>
-      <c r="O28">
-        <v>3.8862206589963547E-2</v>
-      </c>
-      <c r="P28">
-        <v>0.11988417258482574</v>
-      </c>
-      <c r="Q28">
-        <v>3.0471416556105239E-2</v>
-      </c>
-      <c r="R28">
-        <v>1.8361572605862291E-2</v>
+        <v>1.2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="J28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="K28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="L28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="M28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="N28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="O28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="Q28" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="R28" s="2">
+        <v>1.2</v>
       </c>
       <c r="CY28" s="3"/>
     </row>
@@ -2031,55 +2037,55 @@
         <v>28</v>
       </c>
       <c r="B29" s="2">
-        <v>9.7134759000000001E-2</v>
-      </c>
-      <c r="C29" s="4">
-        <v>5.96839869E-2</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0.18498173530000001</v>
+        <v>1.3</v>
+      </c>
+      <c r="C29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="D29" s="2">
+        <v>1.3</v>
       </c>
       <c r="E29" s="2">
-        <v>3.4318872397739252E-2</v>
+        <v>1.3</v>
       </c>
       <c r="F29" s="2">
-        <v>2.8356249568161403E-2</v>
+        <v>1.3</v>
       </c>
       <c r="G29" s="2">
-        <v>8.5857132222069574E-2</v>
+        <v>1.3</v>
       </c>
       <c r="H29" s="2">
-        <v>6.5556520732108825E-2</v>
-      </c>
-      <c r="I29">
-        <v>5.1555813899999997E-2</v>
-      </c>
-      <c r="J29">
-        <v>2.3354884927559067E-2</v>
-      </c>
-      <c r="K29">
-        <v>2.3903379796399914E-2</v>
-      </c>
-      <c r="L29">
-        <v>4.1548518044979194E-2</v>
-      </c>
-      <c r="M29">
-        <v>6.5871310547846645E-2</v>
-      </c>
-      <c r="N29">
-        <v>5.2447734525851282E-2</v>
-      </c>
-      <c r="O29">
-        <v>4.0965767235857875E-2</v>
-      </c>
-      <c r="P29">
-        <v>0.12875372829711618</v>
-      </c>
-      <c r="Q29">
-        <v>3.4480769007259389E-2</v>
-      </c>
-      <c r="R29">
-        <v>2.2119874761375065E-2</v>
+        <v>1.3</v>
+      </c>
+      <c r="I29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="J29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="K29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="L29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="M29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="N29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="O29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>1.3</v>
+      </c>
+      <c r="R29" s="2">
+        <v>1.3</v>
       </c>
       <c r="CZ29" s="3"/>
     </row>
@@ -2088,55 +2094,55 @@
         <v>29</v>
       </c>
       <c r="B30" s="2">
-        <v>0.1080460706</v>
-      </c>
-      <c r="C30" s="4">
-        <v>7.31422558E-2</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0.2227227044</v>
+        <v>1.4</v>
+      </c>
+      <c r="C30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="D30" s="2">
+        <v>1.4</v>
       </c>
       <c r="E30" s="2">
-        <v>3.4852556829523269E-2</v>
+        <v>1.4</v>
       </c>
       <c r="F30" s="2">
-        <v>2.3907081791241663E-2</v>
+        <v>1.4</v>
       </c>
       <c r="G30" s="2">
-        <v>9.1706326619890255E-2</v>
+        <v>1.4</v>
       </c>
       <c r="H30" s="2">
-        <v>6.5351364413129373E-2</v>
-      </c>
-      <c r="I30">
-        <v>4.9466515000000003E-2</v>
-      </c>
-      <c r="J30">
-        <v>2.3554626719801987E-2</v>
-      </c>
-      <c r="K30">
-        <v>2.5264099471947018E-2</v>
-      </c>
-      <c r="L30">
-        <v>4.4266190385653E-2</v>
-      </c>
-      <c r="M30">
-        <v>5.1770694941561099E-2</v>
-      </c>
-      <c r="N30">
-        <v>5.9912969109651749E-2</v>
-      </c>
-      <c r="O30">
-        <v>3.7873064510573359E-2</v>
-      </c>
-      <c r="P30">
-        <v>0.12013529799524524</v>
-      </c>
-      <c r="Q30">
-        <v>2.814496168559116E-2</v>
-      </c>
-      <c r="R30">
-        <v>1.8855396343090046E-2</v>
+        <v>1.4</v>
+      </c>
+      <c r="I30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="J30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="K30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="L30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="M30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="N30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="O30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>1.4</v>
+      </c>
+      <c r="R30" s="2">
+        <v>1.4</v>
       </c>
       <c r="DA30" s="3"/>
     </row>
@@ -2145,55 +2151,55 @@
         <v>30</v>
       </c>
       <c r="B31" s="2">
-        <v>0.10977175290000001</v>
-      </c>
-      <c r="C31" s="4">
-        <v>8.0533735999999995E-2</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0.23990036710000001</v>
+        <v>1.5</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="D31" s="2">
+        <v>1.5</v>
       </c>
       <c r="E31" s="2">
-        <v>3.5006137266876097E-2</v>
+        <v>1.5</v>
       </c>
       <c r="F31" s="2">
-        <v>2.125090908781805E-2</v>
+        <v>1.5</v>
       </c>
       <c r="G31" s="2">
-        <v>9.2990324934754981E-2</v>
+        <v>1.5</v>
       </c>
       <c r="H31" s="2">
-        <v>6.2769177341616467E-2</v>
-      </c>
-      <c r="I31">
-        <v>5.1108602000000003E-2</v>
-      </c>
-      <c r="J31">
-        <v>2.2826238712993205E-2</v>
-      </c>
-      <c r="K31">
-        <v>2.5234529908098335E-2</v>
-      </c>
-      <c r="L31">
-        <v>4.4617851621638061E-2</v>
-      </c>
-      <c r="M31">
-        <v>4.1542653246557995E-2</v>
-      </c>
-      <c r="N31">
-        <v>6.0305910651118746E-2</v>
-      </c>
-      <c r="O31">
-        <v>3.4808141854301609E-2</v>
-      </c>
-      <c r="P31">
-        <v>0.10788706541902324</v>
-      </c>
-      <c r="Q31">
-        <v>2.6551595075997816E-2</v>
-      </c>
-      <c r="R31">
-        <v>1.5072107018316988E-2</v>
+        <v>1.5</v>
+      </c>
+      <c r="I31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="J31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="K31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="L31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="M31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="N31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="O31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="R31" s="2">
+        <v>1.5</v>
       </c>
       <c r="DB31" s="3"/>
     </row>
@@ -2202,55 +2208,55 @@
         <v>31</v>
       </c>
       <c r="B32" s="2">
-        <v>0.1137776689</v>
-      </c>
-      <c r="C32" s="4">
-        <v>9.0698804100000002E-2</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0.2628370478</v>
+        <v>1.6</v>
+      </c>
+      <c r="C32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="D32" s="2">
+        <v>1.6</v>
       </c>
       <c r="E32" s="2">
-        <v>3.3930829531466776E-2</v>
+        <v>1.6</v>
       </c>
       <c r="F32" s="2">
-        <v>1.8558861188557516E-2</v>
+        <v>1.6</v>
       </c>
       <c r="G32" s="2">
-        <v>9.2380534009228479E-2</v>
+        <v>1.6</v>
       </c>
       <c r="H32" s="2">
-        <v>5.9436705333069134E-2</v>
-      </c>
-      <c r="I32">
-        <v>4.8021290199999997E-2</v>
-      </c>
-      <c r="J32">
-        <v>2.2798615818551457E-2</v>
-      </c>
-      <c r="K32">
-        <v>2.551349531066132E-2</v>
-      </c>
-      <c r="L32">
-        <v>4.3266432134630606E-2</v>
-      </c>
-      <c r="M32">
-        <v>3.6301680863592034E-2</v>
-      </c>
-      <c r="N32">
-        <v>5.881918415022E-2</v>
-      </c>
-      <c r="O32">
-        <v>3.6729986726722806E-2</v>
-      </c>
-      <c r="P32">
-        <v>0.10156599449828445</v>
-      </c>
-      <c r="Q32">
-        <v>2.8495900352681756E-2</v>
-      </c>
-      <c r="R32">
-        <v>1.4239098190734309E-2</v>
+        <v>1.6</v>
+      </c>
+      <c r="I32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="J32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="K32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="L32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="M32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="N32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="O32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="P32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="Q32" s="2">
+        <v>1.6</v>
+      </c>
+      <c r="R32" s="2">
+        <v>1.6</v>
       </c>
       <c r="MT32" s="3"/>
     </row>
@@ -2259,55 +2265,55 @@
         <v>32</v>
       </c>
       <c r="B33" s="2">
-        <v>0.1007532148</v>
-      </c>
-      <c r="C33" s="4">
-        <v>9.4993658699999997E-2</v>
-      </c>
-      <c r="D33" s="4">
-        <v>0.25484809470000003</v>
+        <v>1.7</v>
+      </c>
+      <c r="C33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1.7</v>
       </c>
       <c r="E33" s="2">
-        <v>3.262939372493015E-2</v>
+        <v>1.7</v>
       </c>
       <c r="F33" s="2">
-        <v>1.6970392015665126E-2</v>
+        <v>1.7</v>
       </c>
       <c r="G33" s="2">
-        <v>8.6158211737213275E-2</v>
+        <v>1.7</v>
       </c>
       <c r="H33" s="2">
-        <v>5.5247742890302765E-2</v>
-      </c>
-      <c r="I33">
-        <v>4.8555585200000001E-2</v>
-      </c>
-      <c r="J33">
-        <v>2.3206117905210249E-2</v>
-      </c>
-      <c r="K33">
-        <v>2.6212420943379566E-2</v>
-      </c>
-      <c r="L33">
-        <v>3.9385316117624018E-2</v>
-      </c>
-      <c r="M33">
-        <v>3.4914248256545266E-2</v>
-      </c>
-      <c r="N33">
-        <v>4.7358804817759059E-2</v>
-      </c>
-      <c r="O33">
-        <v>4.4729241074414471E-2</v>
-      </c>
-      <c r="P33">
-        <v>9.6817945708750838E-2</v>
-      </c>
-      <c r="Q33">
-        <v>3.221254775097223E-2</v>
-      </c>
-      <c r="R33">
-        <v>1.6806977626090253E-2</v>
+        <v>1.7</v>
+      </c>
+      <c r="I33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="J33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="K33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="L33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="M33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="N33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="O33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="P33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>1.7</v>
+      </c>
+      <c r="R33" s="2">
+        <v>1.7</v>
       </c>
       <c r="MS33" s="3"/>
     </row>
@@ -2316,55 +2322,55 @@
         <v>33</v>
       </c>
       <c r="B34" s="2">
-        <v>8.5512443600000002E-2</v>
-      </c>
-      <c r="C34" s="4">
-        <v>9.3268353999999998E-2</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0.20908736759999999</v>
+        <v>1.8</v>
+      </c>
+      <c r="C34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1.8</v>
       </c>
       <c r="E34" s="2">
-        <v>3.0846762870185059E-2</v>
+        <v>1.8</v>
       </c>
       <c r="F34" s="2">
-        <v>1.6081866587374323E-2</v>
+        <v>1.8</v>
       </c>
       <c r="G34" s="2">
-        <v>7.8029954787529526E-2</v>
+        <v>1.8</v>
       </c>
       <c r="H34" s="2">
-        <v>4.946801476530447E-2</v>
-      </c>
-      <c r="I34">
-        <v>4.7042032300000002E-2</v>
-      </c>
-      <c r="J34">
-        <v>2.3982940265637367E-2</v>
-      </c>
-      <c r="K34">
-        <v>2.6118289447174193E-2</v>
-      </c>
-      <c r="L34">
-        <v>3.5138251844316841E-2</v>
-      </c>
-      <c r="M34">
-        <v>3.8709927271877775E-2</v>
-      </c>
-      <c r="N34">
-        <v>3.9667113476298289E-2</v>
-      </c>
-      <c r="O34">
-        <v>5.3110808879463359E-2</v>
-      </c>
-      <c r="P34">
-        <v>9.2455906697609003E-2</v>
-      </c>
-      <c r="Q34">
-        <v>3.5035046868714788E-2</v>
-      </c>
-      <c r="R34">
-        <v>2.0359916032764179E-2</v>
+        <v>1.8</v>
+      </c>
+      <c r="I34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="J34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="K34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="L34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="M34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="N34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="O34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="P34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>1.8</v>
+      </c>
+      <c r="R34" s="2">
+        <v>1.8</v>
       </c>
       <c r="MR34" s="3"/>
       <c r="PV34" s="3"/>
@@ -2374,55 +2380,55 @@
         <v>34</v>
       </c>
       <c r="B35" s="2">
-        <v>8.4143320999999993E-2</v>
-      </c>
-      <c r="C35" s="4">
-        <v>9.8163211799999997E-2</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0.19836927930000001</v>
+        <v>1.9</v>
+      </c>
+      <c r="C35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="D35" s="2">
+        <v>1.9</v>
       </c>
       <c r="E35" s="2">
-        <v>2.9848094521541003E-2</v>
+        <v>1.9</v>
       </c>
       <c r="F35" s="2">
-        <v>1.5371313286578921E-2</v>
+        <v>1.9</v>
       </c>
       <c r="G35" s="2">
-        <v>7.2350983861880228E-2</v>
+        <v>1.9</v>
       </c>
       <c r="H35" s="2">
-        <v>4.4089757688685893E-2</v>
-      </c>
-      <c r="I35">
-        <v>4.4074279000000001E-2</v>
-      </c>
-      <c r="J35">
-        <v>2.4147623594857736E-2</v>
-      </c>
-      <c r="K35">
-        <v>2.6955965139752826E-2</v>
-      </c>
-      <c r="L35">
-        <v>3.2867224856095299E-2</v>
-      </c>
-      <c r="M35">
-        <v>3.9741097644387442E-2</v>
-      </c>
-      <c r="N35">
-        <v>3.7093081320031043E-2</v>
-      </c>
-      <c r="O35">
-        <v>5.7310239425795322E-2</v>
-      </c>
-      <c r="P35">
-        <v>9.0689609304182101E-2</v>
-      </c>
-      <c r="Q35">
-        <v>3.8559280621499291E-2</v>
-      </c>
-      <c r="R35">
-        <v>2.2692447637275626E-2</v>
+        <v>1.9</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="J35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="K35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="M35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="N35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="O35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="P35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>1.9</v>
+      </c>
+      <c r="R35" s="2">
+        <v>1.9</v>
       </c>
       <c r="MQ35" s="3"/>
       <c r="PU35" s="3"/>
@@ -2432,55 +2438,55 @@
         <v>35</v>
       </c>
       <c r="B36" s="2">
-        <v>8.9140282099999996E-2</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0.1204311025</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0.1864885016</v>
+        <v>2</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
       </c>
       <c r="E36" s="2">
-        <v>2.9260459551371618E-2</v>
+        <v>2</v>
       </c>
       <c r="F36" s="2">
-        <v>1.4325763066031531E-2</v>
+        <v>2</v>
       </c>
       <c r="G36" s="2">
-        <v>7.0630689074948808E-2</v>
+        <v>2</v>
       </c>
       <c r="H36" s="2">
-        <v>4.0085602346268345E-2</v>
-      </c>
-      <c r="I36">
-        <v>4.3075115499999997E-2</v>
-      </c>
-      <c r="J36">
-        <v>2.4259515217855122E-2</v>
-      </c>
-      <c r="K36">
-        <v>2.799679075337716E-2</v>
-      </c>
-      <c r="L36">
-        <v>3.0316486631327993E-2</v>
-      </c>
-      <c r="M36">
-        <v>3.8026332599606222E-2</v>
-      </c>
-      <c r="N36">
-        <v>3.1859615768187965E-2</v>
-      </c>
-      <c r="O36">
-        <v>6.1880206267354222E-2</v>
-      </c>
-      <c r="P36">
-        <v>8.4067896161472852E-2</v>
-      </c>
-      <c r="Q36">
-        <v>3.9979303641297849E-2</v>
-      </c>
-      <c r="R36">
-        <v>2.3839161870019443E-2</v>
+        <v>2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>2</v>
+      </c>
+      <c r="J36" s="2">
+        <v>2</v>
+      </c>
+      <c r="K36" s="2">
+        <v>2</v>
+      </c>
+      <c r="L36" s="2">
+        <v>2</v>
+      </c>
+      <c r="M36" s="2">
+        <v>2</v>
+      </c>
+      <c r="N36" s="2">
+        <v>2</v>
+      </c>
+      <c r="O36" s="2">
+        <v>2</v>
+      </c>
+      <c r="P36" s="2">
+        <v>2</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>2</v>
+      </c>
+      <c r="R36" s="2">
+        <v>2</v>
       </c>
       <c r="AN36" s="1"/>
       <c r="PT36" s="3"/>
@@ -2490,55 +2496,55 @@
         <v>36</v>
       </c>
       <c r="B37" s="2">
-        <v>8.7282312000000001E-2</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0.1194460103</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0.15463816750000001</v>
+        <v>2.1</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2.1</v>
       </c>
       <c r="E37" s="2">
-        <v>2.8408294512894828E-2</v>
+        <v>2.1</v>
       </c>
       <c r="F37" s="2">
-        <v>1.2580334648010455E-2</v>
+        <v>2.1</v>
       </c>
       <c r="G37" s="2">
-        <v>6.5757732246993453E-2</v>
+        <v>2.1</v>
       </c>
       <c r="H37" s="2">
-        <v>3.5837780705131918E-2</v>
-      </c>
-      <c r="I37">
-        <v>3.9075525799999997E-2</v>
-      </c>
-      <c r="J37">
-        <v>2.3543466682103966E-2</v>
-      </c>
-      <c r="K37">
-        <v>2.757695020540565E-2</v>
-      </c>
-      <c r="L37">
-        <v>2.8270217492109496E-2</v>
-      </c>
-      <c r="M37">
-        <v>3.8079782759755987E-2</v>
-      </c>
-      <c r="N37">
-        <v>3.0549809199651966E-2</v>
-      </c>
-      <c r="O37">
-        <v>5.7482656095143705E-2</v>
-      </c>
-      <c r="P37">
-        <v>7.5339122599863112E-2</v>
-      </c>
-      <c r="Q37">
-        <v>3.8386910688721285E-2</v>
-      </c>
-      <c r="R37">
-        <v>2.2919026551385842E-2</v>
+        <v>2.1</v>
+      </c>
+      <c r="I37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="J37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="K37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="L37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="M37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="N37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="O37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="P37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>2.1</v>
+      </c>
+      <c r="R37" s="2">
+        <v>2.1</v>
       </c>
       <c r="GP37" s="3"/>
       <c r="MM37" s="3"/>
@@ -2549,55 +2555,55 @@
         <v>37</v>
       </c>
       <c r="B38" s="2">
-        <v>7.8857596200000005E-2</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0.1196938065</v>
-      </c>
-      <c r="D38" s="4">
-        <v>0.14072539589999999</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2.2000000000000002</v>
       </c>
       <c r="E38" s="2">
-        <v>2.7460732216310336E-2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="F38" s="2">
-        <v>1.1723390304285803E-2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G38" s="2">
-        <v>6.1917798467269115E-2</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="H38" s="2">
-        <v>3.469261461863072E-2</v>
-      </c>
-      <c r="I38">
-        <v>3.5951479199999997E-2</v>
-      </c>
-      <c r="J38">
-        <v>2.337881324126008E-2</v>
-      </c>
-      <c r="K38">
-        <v>2.6629803704727676E-2</v>
-      </c>
-      <c r="L38">
-        <v>2.6386401799486502E-2</v>
-      </c>
-      <c r="M38">
-        <v>4.1255138925096871E-2</v>
-      </c>
-      <c r="N38">
-        <v>3.0025565802583674E-2</v>
-      </c>
-      <c r="O38">
-        <v>4.7113060100073087E-2</v>
-      </c>
-      <c r="P38">
-        <v>6.6841212770966524E-2</v>
-      </c>
-      <c r="Q38">
-        <v>3.9262392706065956E-2</v>
-      </c>
-      <c r="R38">
-        <v>2.1539973617296537E-2</v>
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="I38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="L38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="M38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="N38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="P38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="R38" s="2">
+        <v>2.2000000000000002</v>
       </c>
       <c r="AX38" s="1"/>
       <c r="GO38" s="3"/>
@@ -2608,55 +2614,55 @@
         <v>38</v>
       </c>
       <c r="B39" s="2">
-        <v>6.19303005E-2</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0.11149009579999999</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0.1113087383</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2.2999999999999998</v>
       </c>
       <c r="E39" s="2">
-        <v>2.6245262069726247E-2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="F39" s="2">
-        <v>1.0902495220353938E-2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="G39" s="2">
-        <v>6.2671681727755488E-2</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="H39" s="2">
-        <v>3.4689541497401118E-2</v>
-      </c>
-      <c r="I39">
-        <v>3.6941054100000002E-2</v>
-      </c>
-      <c r="J39">
-        <v>2.2543714334662197E-2</v>
-      </c>
-      <c r="K39">
-        <v>2.5862068966833351E-2</v>
-      </c>
-      <c r="L39">
-        <v>2.3842395482841578E-2</v>
-      </c>
-      <c r="M39">
-        <v>4.3977934333413585E-2</v>
-      </c>
-      <c r="N39">
-        <v>3.0146466079827242E-2</v>
-      </c>
-      <c r="O39">
-        <v>4.8222413581006277E-2</v>
-      </c>
-      <c r="P39">
-        <v>6.0358745122218345E-2</v>
-      </c>
-      <c r="Q39">
-        <v>4.1944217628604584E-2</v>
-      </c>
-      <c r="R39">
-        <v>2.2826380682929991E-2</v>
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="I39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="J39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="M39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="N39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="O39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="P39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="R39" s="2">
+        <v>2.2999999999999998</v>
       </c>
       <c r="GN39" s="3"/>
       <c r="MO39" s="3"/>
@@ -2667,55 +2673,55 @@
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>4.1464613499999997E-2</v>
-      </c>
-      <c r="C40" s="4">
-        <v>8.1104147400000007E-2</v>
-      </c>
-      <c r="D40" s="4">
-        <v>7.0193482000000001E-2</v>
+        <v>2.4</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2.4</v>
       </c>
       <c r="E40" s="2">
-        <v>2.4559413864603575E-2</v>
+        <v>2.4</v>
       </c>
       <c r="F40" s="2">
-        <v>1.0467652047492126E-2</v>
+        <v>2.4</v>
       </c>
       <c r="G40" s="2">
-        <v>5.7938567479095641E-2</v>
+        <v>2.4</v>
       </c>
       <c r="H40" s="2">
-        <v>3.4625281815239217E-2</v>
-      </c>
-      <c r="I40">
-        <v>3.3442735000000001E-2</v>
-      </c>
-      <c r="J40">
-        <v>2.1610962660471085E-2</v>
-      </c>
-      <c r="K40">
-        <v>2.5161877383331543E-2</v>
-      </c>
-      <c r="L40">
-        <v>2.1071835310743241E-2</v>
-      </c>
-      <c r="M40">
-        <v>4.5413354853613037E-2</v>
-      </c>
-      <c r="N40">
-        <v>3.1512414739023976E-2</v>
-      </c>
-      <c r="O40">
-        <v>4.6838845391928896E-2</v>
-      </c>
-      <c r="P40">
-        <v>5.6330360431044148E-2</v>
-      </c>
-      <c r="Q40">
-        <v>4.6181226324748262E-2</v>
-      </c>
-      <c r="R40">
-        <v>2.2932498882944404E-2</v>
+        <v>2.4</v>
+      </c>
+      <c r="I40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="J40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="K40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="L40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="M40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="N40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="O40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="P40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>2.4</v>
+      </c>
+      <c r="R40" s="2">
+        <v>2.4</v>
       </c>
       <c r="GM40" s="3"/>
       <c r="MP40" s="3"/>
@@ -2726,55 +2732,55 @@
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>3.7474201700000001E-2</v>
-      </c>
-      <c r="C41" s="4">
-        <v>7.2543246199999994E-2</v>
-      </c>
-      <c r="D41" s="4">
-        <v>5.6486264699999997E-2</v>
+        <v>2.5</v>
+      </c>
+      <c r="C41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="D41" s="2">
+        <v>2.5</v>
       </c>
       <c r="E41" s="2">
-        <v>2.288314064603578E-2</v>
+        <v>2.5</v>
       </c>
       <c r="F41" s="2">
-        <v>1.2551574094509932E-2</v>
+        <v>2.5</v>
       </c>
       <c r="G41" s="2">
-        <v>5.6126192237743996E-2</v>
+        <v>2.5</v>
       </c>
       <c r="H41" s="2">
-        <v>3.4474045375538429E-2</v>
-      </c>
-      <c r="I41">
-        <v>3.2278331899999999E-2</v>
-      </c>
-      <c r="J41">
-        <v>2.0987212639683072E-2</v>
-      </c>
-      <c r="K41">
-        <v>2.447135751169623E-2</v>
-      </c>
-      <c r="L41">
-        <v>2.0128400428756892E-2</v>
-      </c>
-      <c r="M41">
-        <v>4.9231540988920235E-2</v>
-      </c>
-      <c r="N41">
-        <v>3.3262369307824023E-2</v>
-      </c>
-      <c r="O41">
-        <v>4.8221853436482179E-2</v>
-      </c>
-      <c r="P41">
-        <v>5.0617016898184382E-2</v>
-      </c>
-      <c r="Q41">
-        <v>5.1114471053016634E-2</v>
-      </c>
-      <c r="R41">
-        <v>2.4690484612663603E-2</v>
+        <v>2.5</v>
+      </c>
+      <c r="I41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="J41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="K41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="L41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="M41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="N41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="O41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="P41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="Q41" s="2">
+        <v>2.5</v>
+      </c>
+      <c r="R41" s="2">
+        <v>2.5</v>
       </c>
       <c r="T41" s="1"/>
       <c r="PQ41" s="3"/>
@@ -2784,55 +2790,55 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>3.6949793000000002E-2</v>
-      </c>
-      <c r="C42" s="4">
-        <v>5.9994095099999999E-2</v>
-      </c>
-      <c r="D42" s="4">
-        <v>4.8597328799999999E-2</v>
+        <v>2.6</v>
+      </c>
+      <c r="C42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="D42" s="2">
+        <v>2.6</v>
       </c>
       <c r="E42" s="2">
-        <v>2.2281926867326017E-2</v>
+        <v>2.6</v>
       </c>
       <c r="F42" s="2">
-        <v>1.2833229403625326E-2</v>
+        <v>2.6</v>
       </c>
       <c r="G42" s="2">
-        <v>5.7113076516466195E-2</v>
+        <v>2.6</v>
       </c>
       <c r="H42" s="2">
-        <v>3.5754423567773044E-2</v>
-      </c>
-      <c r="I42">
-        <v>3.3995800100000001E-2</v>
-      </c>
-      <c r="J42">
-        <v>2.0218089959493969E-2</v>
-      </c>
-      <c r="K42">
-        <v>2.4266105742136057E-2</v>
-      </c>
-      <c r="L42">
-        <v>1.8893955664204536E-2</v>
-      </c>
-      <c r="M42">
-        <v>5.5609655017708516E-2</v>
-      </c>
-      <c r="N42">
-        <v>3.601435906436451E-2</v>
-      </c>
-      <c r="O42">
-        <v>6.2792075289568608E-2</v>
-      </c>
-      <c r="P42">
-        <v>4.6377377289502919E-2</v>
-      </c>
-      <c r="Q42">
-        <v>5.5567249000210484E-2</v>
-      </c>
-      <c r="R42">
-        <v>2.541716174961468E-2</v>
+        <v>2.6</v>
+      </c>
+      <c r="I42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="J42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="K42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="L42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="M42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="N42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="O42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="P42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="Q42" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="R42" s="2">
+        <v>2.6</v>
       </c>
       <c r="GI42" s="3"/>
       <c r="PR42" s="3"/>
@@ -2842,55 +2848,55 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>3.9759214000000001E-2</v>
-      </c>
-      <c r="C43" s="4">
-        <v>4.5951461999999998E-2</v>
-      </c>
-      <c r="D43" s="4">
-        <v>4.2716027400000002E-2</v>
+        <v>2.7</v>
+      </c>
+      <c r="C43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="D43" s="2">
+        <v>2.7</v>
       </c>
       <c r="E43" s="2">
-        <v>2.4523166327249459E-2</v>
+        <v>2.7</v>
       </c>
       <c r="F43" s="2">
-        <v>1.4013937148451748E-2</v>
+        <v>2.7</v>
       </c>
       <c r="G43" s="2">
-        <v>5.4112535380150512E-2</v>
+        <v>2.7</v>
       </c>
       <c r="H43" s="2">
-        <v>3.7530777109291806E-2</v>
-      </c>
-      <c r="I43">
-        <v>3.8167410399999997E-2</v>
-      </c>
-      <c r="J43">
-        <v>1.9348173688135194E-2</v>
-      </c>
-      <c r="K43">
-        <v>2.3323238889770385E-2</v>
-      </c>
-      <c r="L43">
-        <v>1.8089090033933476E-2</v>
-      </c>
-      <c r="M43">
-        <v>6.7232525719530686E-2</v>
-      </c>
-      <c r="N43">
-        <v>3.945105227343175E-2</v>
-      </c>
-      <c r="O43">
-        <v>7.054462397323083E-2</v>
-      </c>
-      <c r="P43">
-        <v>4.2382079518221295E-2</v>
-      </c>
-      <c r="Q43">
-        <v>5.4549587085798205E-2</v>
-      </c>
-      <c r="R43">
-        <v>2.4294512183810048E-2</v>
+        <v>2.7</v>
+      </c>
+      <c r="I43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="J43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="K43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="L43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="M43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="N43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="O43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="P43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>2.7</v>
+      </c>
+      <c r="R43" s="2">
+        <v>2.7</v>
       </c>
       <c r="GJ43" s="3"/>
     </row>
@@ -2899,55 +2905,55 @@
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>3.83154473E-2</v>
-      </c>
-      <c r="C44" s="4">
-        <v>4.0106632699999999E-2</v>
-      </c>
-      <c r="D44" s="4">
-        <v>3.8122406599999999E-2</v>
+        <v>2.8</v>
+      </c>
+      <c r="C44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="D44" s="2">
+        <v>2.8</v>
       </c>
       <c r="E44" s="2">
-        <v>2.9461596483200892E-2</v>
+        <v>2.8</v>
       </c>
       <c r="F44" s="2">
-        <v>1.4240751253062374E-2</v>
+        <v>2.8</v>
       </c>
       <c r="G44" s="2">
-        <v>5.4631319094129015E-2</v>
+        <v>2.8</v>
       </c>
       <c r="H44" s="2">
-        <v>3.9614027393797227E-2</v>
-      </c>
-      <c r="I44">
-        <v>4.3036534600000002E-2</v>
-      </c>
-      <c r="J44">
-        <v>1.8621431107333528E-2</v>
-      </c>
-      <c r="K44">
-        <v>2.2142336215469835E-2</v>
-      </c>
-      <c r="L44">
-        <v>1.7267098849224602E-2</v>
-      </c>
-      <c r="M44">
-        <v>8.6583309812453671E-2</v>
-      </c>
-      <c r="N44">
-        <v>4.2973512709943339E-2</v>
-      </c>
-      <c r="O44">
-        <v>7.1445902323140922E-2</v>
-      </c>
-      <c r="P44">
-        <v>3.9755119109478189E-2</v>
-      </c>
-      <c r="Q44">
-        <v>5.2602195893554991E-2</v>
-      </c>
-      <c r="R44">
-        <v>2.1467276828776895E-2</v>
+        <v>2.8</v>
+      </c>
+      <c r="I44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="J44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="K44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="L44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="M44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="N44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="O44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="P44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>2.8</v>
+      </c>
+      <c r="R44" s="2">
+        <v>2.8</v>
       </c>
       <c r="GK44" s="3"/>
     </row>
@@ -2956,55 +2962,55 @@
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>3.0459678E-2</v>
-      </c>
-      <c r="C45" s="4">
-        <v>3.7528052499999999E-2</v>
-      </c>
-      <c r="D45" s="4">
-        <v>3.5658754000000001E-2</v>
+        <v>2.9</v>
+      </c>
+      <c r="C45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="D45" s="2">
+        <v>2.9</v>
       </c>
       <c r="E45" s="2">
-        <v>3.1970756019686991E-2</v>
+        <v>2.9</v>
       </c>
       <c r="F45" s="2">
-        <v>1.3984430669053045E-2</v>
+        <v>2.9</v>
       </c>
       <c r="G45" s="2">
-        <v>4.9078500038342576E-2</v>
+        <v>2.9</v>
       </c>
       <c r="H45" s="2">
-        <v>4.2549264250568694E-2</v>
-      </c>
-      <c r="I45">
-        <v>4.9176269299999999E-2</v>
-      </c>
-      <c r="J45">
-        <v>1.7661077124931555E-2</v>
-      </c>
-      <c r="K45">
-        <v>2.3510870138429757E-2</v>
-      </c>
-      <c r="L45">
-        <v>1.6158652777813545E-2</v>
-      </c>
-      <c r="M45">
-        <v>9.3444496759998011E-2</v>
-      </c>
-      <c r="N45">
-        <v>4.6804710008889576E-2</v>
-      </c>
-      <c r="O45">
-        <v>7.5711320063499815E-2</v>
-      </c>
-      <c r="P45">
-        <v>3.8227982423658789E-2</v>
-      </c>
-      <c r="Q45">
-        <v>5.0660492986517772E-2</v>
-      </c>
-      <c r="R45">
-        <v>1.9652170817238371E-2</v>
+        <v>2.9</v>
+      </c>
+      <c r="I45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="J45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="K45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="L45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="M45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="N45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="O45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="P45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="Q45" s="2">
+        <v>2.9</v>
+      </c>
+      <c r="R45" s="2">
+        <v>2.9</v>
       </c>
       <c r="GL45" s="3"/>
     </row>
@@ -3013,55 +3019,55 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>2.51580868E-2</v>
-      </c>
-      <c r="C46" s="4">
-        <v>2.8550127200000001E-2</v>
-      </c>
-      <c r="D46" s="4">
-        <v>3.5212288100000003E-2</v>
+        <v>3</v>
+      </c>
+      <c r="C46" s="2">
+        <v>3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>3</v>
       </c>
       <c r="E46" s="2">
-        <v>3.3220310807169529E-2</v>
+        <v>3</v>
       </c>
       <c r="F46" s="2">
-        <v>1.7378191563023754E-2</v>
+        <v>3</v>
       </c>
       <c r="G46" s="2">
-        <v>4.1498559076266671E-2</v>
+        <v>3</v>
       </c>
       <c r="H46" s="2">
-        <v>4.4363448780523486E-2</v>
-      </c>
-      <c r="I46">
-        <v>5.1379053500000001E-2</v>
-      </c>
-      <c r="J46">
-        <v>1.703421749885271E-2</v>
-      </c>
-      <c r="K46">
-        <v>2.4026554096925189E-2</v>
-      </c>
-      <c r="L46">
-        <v>1.5638545290013912E-2</v>
-      </c>
-      <c r="M46">
-        <v>9.5794851640771977E-2</v>
-      </c>
-      <c r="N46">
-        <v>4.8755526462926593E-2</v>
-      </c>
-      <c r="O46">
-        <v>6.1415906462803545E-2</v>
-      </c>
-      <c r="P46">
-        <v>3.6699266843012911E-2</v>
-      </c>
-      <c r="Q46">
-        <v>4.75004979040482E-2</v>
-      </c>
-      <c r="R46">
-        <v>1.6196705692665677E-2</v>
+        <v>3</v>
+      </c>
+      <c r="I46" s="2">
+        <v>3</v>
+      </c>
+      <c r="J46" s="2">
+        <v>3</v>
+      </c>
+      <c r="K46" s="2">
+        <v>3</v>
+      </c>
+      <c r="L46" s="2">
+        <v>3</v>
+      </c>
+      <c r="M46" s="2">
+        <v>3</v>
+      </c>
+      <c r="N46" s="2">
+        <v>3</v>
+      </c>
+      <c r="O46" s="2">
+        <v>3</v>
+      </c>
+      <c r="P46" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q46" s="2">
+        <v>3</v>
+      </c>
+      <c r="R46" s="2">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:702" x14ac:dyDescent="0.25">
@@ -3069,55 +3075,55 @@
         <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>1.8990117899999999E-2</v>
-      </c>
-      <c r="C47" s="4">
-        <v>2.65559036E-2</v>
-      </c>
-      <c r="D47" s="4">
-        <v>3.3091885100000003E-2</v>
+        <v>3.1</v>
+      </c>
+      <c r="C47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="D47" s="2">
+        <v>3.1</v>
       </c>
       <c r="E47" s="2">
-        <v>3.2218376932932023E-2</v>
+        <v>3.1</v>
       </c>
       <c r="F47" s="2">
-        <v>1.6638797712681407E-2</v>
+        <v>3.1</v>
       </c>
       <c r="G47" s="2">
-        <v>4.1866465447995521E-2</v>
+        <v>3.1</v>
       </c>
       <c r="H47" s="2">
-        <v>4.5346962522183933E-2</v>
-      </c>
-      <c r="I47">
-        <v>4.7110778300000003E-2</v>
-      </c>
-      <c r="J47">
-        <v>1.695331775606046E-2</v>
-      </c>
-      <c r="K47">
-        <v>2.4208940342351708E-2</v>
-      </c>
-      <c r="L47">
-        <v>1.5331344395547591E-2</v>
-      </c>
-      <c r="M47">
-        <v>9.5019395351288768E-2</v>
-      </c>
-      <c r="N47">
-        <v>4.556984270968277E-2</v>
-      </c>
-      <c r="O47">
-        <v>5.3250272011651271E-2</v>
-      </c>
-      <c r="P47">
-        <v>3.498103025571489E-2</v>
-      </c>
-      <c r="Q47">
-        <v>4.5657136650250806E-2</v>
-      </c>
-      <c r="R47">
-        <v>1.5427804829574071E-2</v>
+        <v>3.1</v>
+      </c>
+      <c r="I47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="J47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="K47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="L47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="M47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="N47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="O47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="P47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="Q47" s="2">
+        <v>3.1</v>
+      </c>
+      <c r="R47" s="2">
+        <v>3.1</v>
       </c>
       <c r="ZZ47" s="3"/>
     </row>
@@ -3126,55 +3132,55 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>1.48537991E-2</v>
-      </c>
-      <c r="C48" s="4">
-        <v>2.4804390999999999E-2</v>
-      </c>
-      <c r="D48" s="4">
-        <v>2.7486161499999998E-2</v>
+        <v>3.2</v>
+      </c>
+      <c r="C48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="D48" s="2">
+        <v>3.2</v>
       </c>
       <c r="E48" s="2">
-        <v>2.807038215459727E-2</v>
+        <v>3.2</v>
       </c>
       <c r="F48" s="2">
-        <v>1.3612747902632191E-2</v>
+        <v>3.2</v>
       </c>
       <c r="G48" s="2">
-        <v>3.9616532283664532E-2</v>
+        <v>3.2</v>
       </c>
       <c r="H48" s="2">
-        <v>4.6796947905802272E-2</v>
-      </c>
-      <c r="I48">
-        <v>4.8813986699999999E-2</v>
-      </c>
-      <c r="J48">
-        <v>1.6273465756425558E-2</v>
-      </c>
-      <c r="K48">
-        <v>2.386081926396966E-2</v>
-      </c>
-      <c r="L48">
-        <v>1.5016085191590355E-2</v>
-      </c>
-      <c r="M48">
-        <v>9.8017331664913845E-2</v>
-      </c>
-      <c r="N48">
-        <v>4.0230770940595392E-2</v>
-      </c>
-      <c r="O48">
-        <v>5.4945760323032826E-2</v>
-      </c>
-      <c r="P48">
-        <v>3.2977841734863782E-2</v>
-      </c>
-      <c r="Q48">
-        <v>3.7280187568895964E-2</v>
-      </c>
-      <c r="R48">
-        <v>1.6515507071727907E-2</v>
+        <v>3.2</v>
+      </c>
+      <c r="I48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="J48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="K48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="L48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="M48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="N48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="O48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="P48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="Q48" s="2">
+        <v>3.2</v>
+      </c>
+      <c r="R48" s="2">
+        <v>3.2</v>
       </c>
       <c r="ZY48" s="3"/>
     </row>
@@ -3183,55 +3189,55 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>1.6463022500000001E-2</v>
-      </c>
-      <c r="C49" s="4">
-        <v>2.1873026800000001E-2</v>
-      </c>
-      <c r="D49" s="4">
-        <v>2.54142825E-2</v>
+        <v>3.3</v>
+      </c>
+      <c r="C49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="D49" s="2">
+        <v>3.3</v>
       </c>
       <c r="E49" s="2">
-        <v>2.7761515329587146E-2</v>
+        <v>3.3</v>
       </c>
       <c r="F49" s="2">
-        <v>1.2418365876104625E-2</v>
+        <v>3.3</v>
       </c>
       <c r="G49" s="2">
-        <v>3.5690531476611796E-2</v>
+        <v>3.3</v>
       </c>
       <c r="H49" s="2">
-        <v>4.6558355790932718E-2</v>
-      </c>
-      <c r="I49">
-        <v>5.0673253100000003E-2</v>
-      </c>
-      <c r="J49">
-        <v>1.5578628354654461E-2</v>
-      </c>
-      <c r="K49">
-        <v>2.286815164277314E-2</v>
-      </c>
-      <c r="L49">
-        <v>1.4630701832263166E-2</v>
-      </c>
-      <c r="M49">
-        <v>9.8591935818221288E-2</v>
-      </c>
-      <c r="N49">
-        <v>3.6240934357490123E-2</v>
-      </c>
-      <c r="O49">
-        <v>5.4312619318257101E-2</v>
-      </c>
-      <c r="P49">
-        <v>3.2086503476365075E-2</v>
-      </c>
-      <c r="Q49">
-        <v>2.7733196375716352E-2</v>
-      </c>
-      <c r="R49">
-        <v>1.7255832544331023E-2</v>
+        <v>3.3</v>
+      </c>
+      <c r="I49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="J49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="K49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="L49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="M49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="N49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="O49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="P49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="Q49" s="2">
+        <v>3.3</v>
+      </c>
+      <c r="R49" s="2">
+        <v>3.3</v>
       </c>
       <c r="ZX49" s="3"/>
     </row>
@@ -3240,55 +3246,55 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>1.67931591E-2</v>
-      </c>
-      <c r="C50" s="4">
-        <v>1.9986000100000002E-2</v>
-      </c>
-      <c r="D50" s="4">
-        <v>2.1095941600000001E-2</v>
+        <v>3.4</v>
+      </c>
+      <c r="C50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="D50" s="2">
+        <v>3.4</v>
       </c>
       <c r="E50" s="2">
-        <v>2.824745703677118E-2</v>
+        <v>3.4</v>
       </c>
       <c r="F50" s="2">
-        <v>1.2520785017454508E-2</v>
+        <v>3.4</v>
       </c>
       <c r="G50" s="2">
-        <v>3.5920740859194986E-2</v>
+        <v>3.4</v>
       </c>
       <c r="H50" s="2">
-        <v>4.5226367024361336E-2</v>
-      </c>
-      <c r="I50">
-        <v>5.3938839400000001E-2</v>
-      </c>
-      <c r="J50">
-        <v>1.4802057603843278E-2</v>
-      </c>
-      <c r="K50">
-        <v>2.2161668346775937E-2</v>
-      </c>
-      <c r="L50">
-        <v>1.3886126865494626E-2</v>
-      </c>
-      <c r="M50">
-        <v>9.140582592333045E-2</v>
-      </c>
-      <c r="N50">
-        <v>3.3908201719445516E-2</v>
-      </c>
-      <c r="O50">
-        <v>5.4865771807473103E-2</v>
-      </c>
-      <c r="P50">
-        <v>3.171171171425119E-2</v>
-      </c>
-      <c r="Q50">
-        <v>1.9865450321564622E-2</v>
-      </c>
-      <c r="R50">
-        <v>2.0531043326947516E-2</v>
+        <v>3.4</v>
+      </c>
+      <c r="I50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="J50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="K50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="L50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="M50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="N50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="O50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="P50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="Q50" s="2">
+        <v>3.4</v>
+      </c>
+      <c r="R50" s="2">
+        <v>3.4</v>
       </c>
       <c r="ZW50" s="3"/>
     </row>
@@ -3297,55 +3303,55 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>1.7680400799999999E-2</v>
-      </c>
-      <c r="C51" s="4">
-        <v>1.76000789E-2</v>
-      </c>
-      <c r="D51" s="4">
-        <v>1.61470147E-2</v>
+        <v>3.5</v>
+      </c>
+      <c r="C51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="D51" s="2">
+        <v>3.5</v>
       </c>
       <c r="E51" s="2">
-        <v>2.8706447931263802E-2</v>
+        <v>3.5</v>
       </c>
       <c r="F51" s="2">
-        <v>1.2436023014991561E-2</v>
+        <v>3.5</v>
       </c>
       <c r="G51" s="2">
-        <v>3.7428803905614323E-2</v>
+        <v>3.5</v>
       </c>
       <c r="H51" s="2">
-        <v>4.3359115126117009E-2</v>
-      </c>
-      <c r="I51">
-        <v>5.7861556100000003E-2</v>
-      </c>
-      <c r="J51">
-        <v>1.3401612551754195E-2</v>
-      </c>
-      <c r="K51">
-        <v>2.0928390268551738E-2</v>
-      </c>
-      <c r="L51">
-        <v>1.2939562740295193E-2</v>
-      </c>
-      <c r="M51">
-        <v>9.0185702594007211E-2</v>
-      </c>
-      <c r="N51">
-        <v>3.3008104524559219E-2</v>
-      </c>
-      <c r="O51">
-        <v>5.8685587151857073E-2</v>
-      </c>
-      <c r="P51">
-        <v>3.3556371468936898E-2</v>
-      </c>
-      <c r="Q51">
-        <v>2.0331151325324429E-2</v>
-      </c>
-      <c r="R51">
-        <v>2.3261897581443779E-2</v>
+        <v>3.5</v>
+      </c>
+      <c r="I51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="J51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="K51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="L51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="M51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="N51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="O51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="P51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="Q51" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="R51" s="2">
+        <v>3.5</v>
       </c>
       <c r="CE51" s="1"/>
     </row>
@@ -3354,55 +3360,55 @@
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>1.7954326699999999E-2</v>
-      </c>
-      <c r="C52" s="4">
-        <v>1.4593781300000001E-2</v>
-      </c>
-      <c r="D52" s="4">
-        <v>1.32188711E-2</v>
+        <v>3.6</v>
+      </c>
+      <c r="C52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="D52" s="2">
+        <v>3.6</v>
       </c>
       <c r="E52" s="2">
-        <v>2.9750897119539609E-2</v>
+        <v>3.6</v>
       </c>
       <c r="F52" s="2">
-        <v>1.3752106635667486E-2</v>
+        <v>3.6</v>
       </c>
       <c r="G52" s="2">
-        <v>4.1484859413817653E-2</v>
+        <v>3.6</v>
       </c>
       <c r="H52" s="2">
-        <v>4.1970828979925663E-2</v>
-      </c>
-      <c r="I52">
-        <v>6.0559357199999997E-2</v>
-      </c>
-      <c r="J52">
-        <v>1.3166939276453547E-2</v>
-      </c>
-      <c r="K52">
-        <v>2.00719392529797E-2</v>
-      </c>
-      <c r="L52">
-        <v>1.2253872262817543E-2</v>
-      </c>
-      <c r="M52">
-        <v>9.5270600516298862E-2</v>
-      </c>
-      <c r="N52">
-        <v>3.2849065419076166E-2</v>
-      </c>
-      <c r="O52">
-        <v>4.5948734227478735E-2</v>
-      </c>
-      <c r="P52">
-        <v>3.4384027510821508E-2</v>
-      </c>
-      <c r="Q52">
-        <v>2.3696483337053657E-2</v>
-      </c>
-      <c r="R52">
-        <v>2.4214068784371667E-2</v>
+        <v>3.6</v>
+      </c>
+      <c r="I52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="J52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="K52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="L52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="M52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="N52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="O52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="P52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="Q52" s="2">
+        <v>3.6</v>
+      </c>
+      <c r="R52" s="2">
+        <v>3.6</v>
       </c>
       <c r="ZS52" s="3"/>
     </row>
@@ -3411,55 +3417,55 @@
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>1.6413244300000001E-2</v>
-      </c>
-      <c r="C53" s="4">
-        <v>1.02481741E-2</v>
-      </c>
-      <c r="D53" s="4">
-        <v>1.11794298E-2</v>
+        <v>3.7</v>
+      </c>
+      <c r="C53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="D53" s="2">
+        <v>3.7</v>
       </c>
       <c r="E53" s="2">
-        <v>3.1390486226129131E-2</v>
+        <v>3.7</v>
       </c>
       <c r="F53" s="2">
-        <v>1.3876089570759712E-2</v>
+        <v>3.7</v>
       </c>
       <c r="G53" s="2">
-        <v>4.6729556732209819E-2</v>
+        <v>3.7</v>
       </c>
       <c r="H53" s="2">
-        <v>4.1392395637442639E-2</v>
-      </c>
-      <c r="I53">
-        <v>6.2025600600000001E-2</v>
-      </c>
-      <c r="J53">
-        <v>1.2557165409894648E-2</v>
-      </c>
-      <c r="K53">
-        <v>1.917996407226286E-2</v>
-      </c>
-      <c r="L53">
-        <v>1.1638085700490269E-2</v>
-      </c>
-      <c r="M53">
-        <v>9.7339978319596912E-2</v>
-      </c>
-      <c r="N53">
-        <v>3.5394293178183323E-2</v>
-      </c>
-      <c r="O53">
-        <v>3.6285097189374824E-2</v>
-      </c>
-      <c r="P53">
-        <v>3.3978017443447001E-2</v>
-      </c>
-      <c r="Q53">
-        <v>2.8538760581484336E-2</v>
-      </c>
-      <c r="R53">
-        <v>2.4073725785217229E-2</v>
+        <v>3.7</v>
+      </c>
+      <c r="I53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="J53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="K53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="L53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="M53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="N53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="O53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="P53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="Q53" s="2">
+        <v>3.7</v>
+      </c>
+      <c r="R53" s="2">
+        <v>3.7</v>
       </c>
       <c r="ZT53" s="3"/>
     </row>
@@ -3468,55 +3474,55 @@
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>1.8331024200000001E-2</v>
-      </c>
-      <c r="C54" s="4">
-        <v>9.8107918999999991E-3</v>
-      </c>
-      <c r="D54" s="4">
-        <v>7.2400920000000001E-3</v>
+        <v>3.8</v>
+      </c>
+      <c r="C54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="D54" s="2">
+        <v>3.8</v>
       </c>
       <c r="E54" s="2">
-        <v>3.22353959524838E-2</v>
+        <v>3.8</v>
       </c>
       <c r="F54" s="2">
-        <v>1.365215661800258E-2</v>
+        <v>3.8</v>
       </c>
       <c r="G54" s="2">
-        <v>4.6819384862779576E-2</v>
+        <v>3.8</v>
       </c>
       <c r="H54" s="2">
-        <v>4.0864566975493136E-2</v>
-      </c>
-      <c r="I54">
-        <v>6.1850636700000003E-2</v>
-      </c>
-      <c r="J54">
-        <v>1.1646045666970658E-2</v>
-      </c>
-      <c r="K54">
-        <v>1.8998603724408415E-2</v>
-      </c>
-      <c r="L54">
-        <v>1.1048300148501089E-2</v>
-      </c>
-      <c r="M54">
-        <v>9.450103108099954E-2</v>
-      </c>
-      <c r="N54">
-        <v>3.8765307795613352E-2</v>
-      </c>
-      <c r="O54">
-        <v>3.228167342495715E-2</v>
-      </c>
-      <c r="P54">
-        <v>3.4964512514008221E-2</v>
-      </c>
-      <c r="Q54">
-        <v>2.7918027918027919E-2</v>
-      </c>
-      <c r="R54">
-        <v>2.0606362885573021E-2</v>
+        <v>3.8</v>
+      </c>
+      <c r="I54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="J54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="K54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="L54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="M54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="N54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="O54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="P54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="Q54" s="2">
+        <v>3.8</v>
+      </c>
+      <c r="R54" s="2">
+        <v>3.8</v>
       </c>
       <c r="VZ54" s="3"/>
       <c r="WH54" s="3"/>
@@ -3527,55 +3533,55 @@
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>1.8985644600000001E-2</v>
-      </c>
-      <c r="C55" s="4">
-        <v>1.0897031E-2</v>
-      </c>
-      <c r="D55" s="4">
-        <v>8.5395746000000005E-3</v>
+        <v>3.9</v>
+      </c>
+      <c r="C55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="D55" s="2">
+        <v>3.9</v>
       </c>
       <c r="E55" s="2">
-        <v>3.4966329090856924E-2</v>
+        <v>3.9</v>
       </c>
       <c r="F55" s="2">
-        <v>1.3118796046553258E-2</v>
+        <v>3.9</v>
       </c>
       <c r="G55" s="2">
-        <v>4.7696392703384438E-2</v>
+        <v>3.9</v>
       </c>
       <c r="H55" s="2">
-        <v>4.186140387216835E-2</v>
-      </c>
-      <c r="I55">
-        <v>5.88284102E-2</v>
-      </c>
-      <c r="J55">
-        <v>1.0981504160061717E-2</v>
-      </c>
-      <c r="K55">
-        <v>1.8213444221877664E-2</v>
-      </c>
-      <c r="L55">
-        <v>1.1172136640974765E-2</v>
-      </c>
-      <c r="M55">
-        <v>9.1263866672576133E-2</v>
-      </c>
-      <c r="N55">
-        <v>4.0073506325551143E-2</v>
-      </c>
-      <c r="O55">
-        <v>2.4703087885985749E-2</v>
-      </c>
-      <c r="P55">
-        <v>3.5735394969907346E-2</v>
-      </c>
-      <c r="Q55">
-        <v>2.2591576569307728E-2</v>
-      </c>
-      <c r="R55">
-        <v>1.8430508872855262E-2</v>
+        <v>3.9</v>
+      </c>
+      <c r="I55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="J55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="K55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="L55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="M55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="N55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="O55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="P55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="Q55" s="2">
+        <v>3.9</v>
+      </c>
+      <c r="R55" s="2">
+        <v>3.9</v>
       </c>
       <c r="VY55" s="3"/>
       <c r="WG55" s="3"/>
@@ -3586,55 +3592,55 @@
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>2.04680725E-2</v>
-      </c>
-      <c r="C56" s="4">
-        <v>8.1141280999999996E-3</v>
-      </c>
-      <c r="D56" s="4">
-        <v>1.1245569E-2</v>
+        <v>4</v>
+      </c>
+      <c r="C56" s="2">
+        <v>4</v>
+      </c>
+      <c r="D56" s="2">
+        <v>4</v>
       </c>
       <c r="E56" s="2">
-        <v>3.7168744358838317E-2</v>
+        <v>4</v>
       </c>
       <c r="F56" s="2">
-        <v>1.2947966088816286E-2</v>
+        <v>4</v>
       </c>
       <c r="G56" s="2">
-        <v>5.1371630241191707E-2</v>
+        <v>4</v>
       </c>
       <c r="H56" s="2">
-        <v>4.3836661436944362E-2</v>
-      </c>
-      <c r="I56">
-        <v>5.908559E-2</v>
-      </c>
-      <c r="J56">
-        <v>1.0595275625531954E-2</v>
-      </c>
-      <c r="K56">
-        <v>1.879474031385666E-2</v>
-      </c>
-      <c r="L56">
-        <v>1.1567176490792985E-2</v>
-      </c>
-      <c r="M56">
-        <v>9.4883782887024606E-2</v>
-      </c>
-      <c r="N56">
-        <v>4.2422729111191826E-2</v>
-      </c>
-      <c r="O56">
-        <v>2.6697103944614498E-2</v>
-      </c>
-      <c r="P56">
-        <v>3.8167452402076897E-2</v>
-      </c>
-      <c r="Q56">
-        <v>1.7504959734506952E-2</v>
-      </c>
-      <c r="R56">
-        <v>1.5502851736506529E-2</v>
+        <v>4</v>
+      </c>
+      <c r="I56" s="2">
+        <v>4</v>
+      </c>
+      <c r="J56" s="2">
+        <v>4</v>
+      </c>
+      <c r="K56" s="2">
+        <v>4</v>
+      </c>
+      <c r="L56" s="2">
+        <v>4</v>
+      </c>
+      <c r="M56" s="2">
+        <v>4</v>
+      </c>
+      <c r="N56" s="2">
+        <v>4</v>
+      </c>
+      <c r="O56" s="2">
+        <v>4</v>
+      </c>
+      <c r="P56" s="2">
+        <v>4</v>
+      </c>
+      <c r="Q56" s="2">
+        <v>4</v>
+      </c>
+      <c r="R56" s="2">
+        <v>4</v>
       </c>
       <c r="VX56" s="3"/>
       <c r="WF56" s="3"/>
@@ -3644,55 +3650,55 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>2.2341745999999999E-2</v>
-      </c>
-      <c r="C57" s="4">
-        <v>8.4343700999999997E-3</v>
-      </c>
-      <c r="D57" s="4">
-        <v>9.6202531999999997E-3</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="C57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="D57" s="2">
+        <v>4.0999999999999996</v>
       </c>
       <c r="E57" s="2">
-        <v>3.9706849889502363E-2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="F57" s="2">
-        <v>1.3974933280836002E-2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="G57" s="2">
-        <v>5.7263100920452524E-2</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="H57" s="2">
-        <v>4.5323788502966179E-2</v>
-      </c>
-      <c r="I57">
-        <v>6.4876565600000005E-2</v>
-      </c>
-      <c r="J57">
-        <v>1.0410457296873048E-2</v>
-      </c>
-      <c r="K57">
-        <v>1.884551045311654E-2</v>
-      </c>
-      <c r="L57">
-        <v>1.2299080178530795E-2</v>
-      </c>
-      <c r="M57">
-        <v>9.5277012647898299E-2</v>
-      </c>
-      <c r="N57">
-        <v>4.5605746460331421E-2</v>
-      </c>
-      <c r="O57">
-        <v>2.8432275896220941E-2</v>
-      </c>
-      <c r="P57">
-        <v>4.2303569062503765E-2</v>
-      </c>
-      <c r="Q57">
-        <v>1.2235534030047832E-2</v>
-      </c>
-      <c r="R57">
-        <v>1.5033108632110909E-2</v>
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="I57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="J57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="L57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="M57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="N57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="P57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="Q57" s="2">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="R57" s="2">
+        <v>4.0999999999999996</v>
       </c>
       <c r="VW57" s="3"/>
       <c r="WE57" s="3"/>
@@ -3702,55 +3708,55 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>2.5445419100000002E-2</v>
-      </c>
-      <c r="C58" s="4">
-        <v>1.05667231E-2</v>
-      </c>
-      <c r="D58" s="4">
-        <v>1.3368388199999999E-2</v>
+        <v>4.2</v>
+      </c>
+      <c r="C58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="D58" s="2">
+        <v>4.2</v>
       </c>
       <c r="E58" s="2">
-        <v>4.3441115597902563E-2</v>
+        <v>4.2</v>
       </c>
       <c r="F58" s="2">
-        <v>1.6245993531301999E-2</v>
+        <v>4.2</v>
       </c>
       <c r="G58" s="2">
-        <v>6.1732180371156853E-2</v>
+        <v>4.2</v>
       </c>
       <c r="H58" s="2">
-        <v>4.8599147484263923E-2</v>
-      </c>
-      <c r="I58">
-        <v>7.4687247200000001E-2</v>
-      </c>
-      <c r="J58">
-        <v>1.0405867193326084E-2</v>
-      </c>
-      <c r="K58">
-        <v>2.0289181110477419E-2</v>
-      </c>
-      <c r="L58">
-        <v>1.3926672823021029E-2</v>
-      </c>
-      <c r="M58">
-        <v>9.2500113132602327E-2</v>
-      </c>
-      <c r="N58">
-        <v>4.924444944105183E-2</v>
-      </c>
-      <c r="O58">
-        <v>3.0446773303916159E-2</v>
-      </c>
-      <c r="P58">
-        <v>4.3942092366133001E-2</v>
-      </c>
-      <c r="Q58">
-        <v>1.4848422355124768E-2</v>
-      </c>
-      <c r="R58">
-        <v>1.5062572809176552E-2</v>
+        <v>4.2</v>
+      </c>
+      <c r="I58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="J58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="K58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="L58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="M58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="N58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="O58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="P58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>4.2</v>
+      </c>
+      <c r="R58" s="2">
+        <v>4.2</v>
       </c>
       <c r="BR58" s="1"/>
       <c r="BS58" s="1"/>
@@ -3760,55 +3766,55 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>2.6593343500000002E-2</v>
-      </c>
-      <c r="C59" s="4">
-        <v>1.06797197E-2</v>
-      </c>
-      <c r="D59" s="4">
-        <v>1.3941168300000001E-2</v>
+        <v>4.3</v>
+      </c>
+      <c r="C59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="D59" s="2">
+        <v>4.3</v>
       </c>
       <c r="E59" s="2">
-        <v>4.6547061406434616E-2</v>
+        <v>4.3</v>
       </c>
       <c r="F59" s="2">
-        <v>1.6045051422588354E-2</v>
+        <v>4.3</v>
       </c>
       <c r="G59" s="2">
-        <v>6.5814296846163314E-2</v>
+        <v>4.3</v>
       </c>
       <c r="H59" s="2">
-        <v>5.2850341440579568E-2</v>
-      </c>
-      <c r="I59">
-        <v>8.6669559699999996E-2</v>
-      </c>
-      <c r="J59">
-        <v>1.0253707020993423E-2</v>
-      </c>
-      <c r="K59">
-        <v>2.3376122173317773E-2</v>
-      </c>
-      <c r="L59">
-        <v>1.4977908693660166E-2</v>
-      </c>
-      <c r="M59">
-        <v>8.8265366109544635E-2</v>
-      </c>
-      <c r="N59">
-        <v>5.3870322097475797E-2</v>
-      </c>
-      <c r="O59">
-        <v>2.9404925863771841E-2</v>
-      </c>
-      <c r="P59">
-        <v>4.636131472254279E-2</v>
-      </c>
-      <c r="Q59">
-        <v>1.7808117538861204E-2</v>
-      </c>
-      <c r="R59">
-        <v>1.4993714529734855E-2</v>
+        <v>4.3</v>
+      </c>
+      <c r="I59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="J59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="K59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="L59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="M59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="N59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="O59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="P59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>4.3</v>
+      </c>
+      <c r="R59" s="2">
+        <v>4.3</v>
       </c>
       <c r="MT59" s="3"/>
       <c r="VS59" s="3"/>
@@ -3819,55 +3825,55 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>2.5251321300000001E-2</v>
-      </c>
-      <c r="C60" s="4">
-        <v>1.17946054E-2</v>
-      </c>
-      <c r="D60" s="4">
-        <v>1.51768098E-2</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="D60" s="2">
+        <v>4.4000000000000004</v>
       </c>
       <c r="E60" s="2">
-        <v>4.8142406045552165E-2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="F60" s="2">
-        <v>1.6396051736617675E-2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="G60" s="2">
-        <v>6.6505699050980485E-2</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H60" s="2">
-        <v>5.5280283466362747E-2</v>
-      </c>
-      <c r="I60">
-        <v>8.97156281E-2</v>
-      </c>
-      <c r="J60">
-        <v>1.0332359080811881E-2</v>
-      </c>
-      <c r="K60">
-        <v>2.3766903040657053E-2</v>
-      </c>
-      <c r="L60">
-        <v>1.5566870079042958E-2</v>
-      </c>
-      <c r="M60">
-        <v>8.9659095831560218E-2</v>
-      </c>
-      <c r="N60">
-        <v>5.8367905458519491E-2</v>
-      </c>
-      <c r="O60">
-        <v>2.6832143102902852E-2</v>
-      </c>
-      <c r="P60">
-        <v>4.8631406546350661E-2</v>
-      </c>
-      <c r="Q60">
-        <v>2.2204344335383538E-2</v>
-      </c>
-      <c r="R60">
-        <v>1.5416096132257211E-2</v>
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="I60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="J60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="K60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="L60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="M60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="N60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="O60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="P60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="R60" s="2">
+        <v>4.4000000000000004</v>
       </c>
       <c r="MS60" s="3"/>
       <c r="VT60" s="3"/>
@@ -3878,55 +3884,55 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>3.0799957100000001E-2</v>
+        <v>4.5</v>
       </c>
       <c r="C61" s="2">
-        <v>1.5823951499999999E-2</v>
-      </c>
-      <c r="D61" s="4">
-        <v>1.9293638500000002E-2</v>
+        <v>4.5</v>
+      </c>
+      <c r="D61" s="2">
+        <v>4.5</v>
       </c>
       <c r="E61" s="2">
-        <v>5.0535321187623994E-2</v>
+        <v>4.5</v>
       </c>
       <c r="F61" s="2">
-        <v>1.6600247354679125E-2</v>
+        <v>4.5</v>
       </c>
       <c r="G61" s="2">
-        <v>6.8557930215854559E-2</v>
+        <v>4.5</v>
       </c>
       <c r="H61" s="2">
-        <v>5.6413596924087921E-2</v>
-      </c>
-      <c r="I61">
-        <v>9.4291537699999997E-2</v>
-      </c>
-      <c r="J61">
-        <v>1.1507253728546718E-2</v>
-      </c>
-      <c r="K61">
-        <v>2.4579086656824838E-2</v>
-      </c>
-      <c r="L61">
-        <v>1.6011474595906659E-2</v>
-      </c>
-      <c r="M61">
-        <v>9.1769880352621305E-2</v>
-      </c>
-      <c r="N61">
-        <v>5.974749651142925E-2</v>
-      </c>
-      <c r="O61">
-        <v>2.3952507960023545E-2</v>
-      </c>
-      <c r="P61">
-        <v>4.730027355871607E-2</v>
-      </c>
-      <c r="Q61">
-        <v>2.2658999226756193E-2</v>
-      </c>
-      <c r="R61">
-        <v>1.7409617404191034E-2</v>
+        <v>4.5</v>
+      </c>
+      <c r="I61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="J61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="K61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="L61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="M61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="N61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="O61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="P61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="R61" s="2">
+        <v>4.5</v>
       </c>
       <c r="MR61" s="3"/>
       <c r="VU61" s="3"/>
@@ -3937,16 +3943,55 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>3.32645887E-2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="C62" s="2">
-        <v>1.6659033699999999E-2</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="D62" s="2">
-        <v>1.9646824899999998E-2</v>
-      </c>
-      <c r="I62">
-        <v>9.6183632800000002E-2</v>
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="E62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="F62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="G62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="H62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="J62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="K62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="L62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="M62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="N62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="O62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="P62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="R62" s="2">
+        <v>4.5999999999999996</v>
       </c>
       <c r="MQ62" s="3"/>
       <c r="VV62" s="3"/>
@@ -3957,16 +4002,55 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>3.4891613100000003E-2</v>
+        <v>4.7</v>
       </c>
       <c r="C63" s="2">
-        <v>1.62362697E-2</v>
+        <v>4.7</v>
       </c>
       <c r="D63" s="2">
-        <v>2.48681236E-2</v>
-      </c>
-      <c r="I63">
-        <v>8.2302593800000004E-2</v>
+        <v>4.7</v>
+      </c>
+      <c r="E63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="F63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="G63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="H63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="I63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="J63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="K63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="L63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="M63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="N63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="O63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="P63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="Q63" s="2">
+        <v>4.7</v>
+      </c>
+      <c r="R63" s="2">
+        <v>4.7</v>
       </c>
       <c r="AN63" s="1"/>
     </row>
@@ -3975,16 +4059,55 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>4.0132114000000003E-2</v>
+        <v>4.8</v>
       </c>
       <c r="C64" s="2">
-        <v>1.52230352E-2</v>
+        <v>4.8</v>
       </c>
       <c r="D64" s="2">
-        <v>1.8015854000000001E-2</v>
-      </c>
-      <c r="I64">
-        <v>8.3355183799999996E-2</v>
+        <v>4.8</v>
+      </c>
+      <c r="E64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="F64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="G64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="H64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="I64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="J64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="K64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="L64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="M64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="N64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="O64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="P64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>4.8</v>
+      </c>
+      <c r="R64" s="2">
+        <v>4.8</v>
       </c>
       <c r="MM64" s="3"/>
     </row>

</xml_diff>